<commit_message>
Permission Sets are able to Parse
</commit_message>
<xml_diff>
--- a/backend/changes.xlsx
+++ b/backend/changes.xlsx
@@ -397,14 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>field</v>
+        <v>path</v>
       </c>
       <c r="B1" t="str">
         <v>change</v>
@@ -415,106 +415,425 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>applicationVisibilities.JobApps__Recruiting</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.API_Status__c</v>
       </c>
       <c r="B2" t="str">
-        <v>Unchanged</v>
+        <v>Modified</v>
       </c>
       <c r="C2" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>applicationVisibilities.JobApps__Recruiting1</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.API_Type__c</v>
       </c>
       <c r="B3" t="str">
-        <v>Created</v>
+        <v>Modified</v>
       </c>
       <c r="C3" t="str">
-        <v>Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>userPermissions.ApiEnabled</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.Date_and_Time_of_Submission_Failure__c</v>
       </c>
       <c r="B4" t="str">
-        <v>Unchanged</v>
+        <v>Modified</v>
       </c>
       <c r="C4" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>objectPermissions.Job_Request__c</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.DML_Operation__c</v>
       </c>
       <c r="B5" t="str">
-        <v>Changed</v>
+        <v>Modified</v>
       </c>
       <c r="C5" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>fieldPermissions.Job_Request__c.Salary__c</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.Destination__c</v>
       </c>
       <c r="B6" t="str">
-        <v>Unchanged</v>
+        <v>Modified</v>
       </c>
       <c r="C6" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>pageAccesses.Job_Request_Web_Form</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.Endpoint__c</v>
       </c>
       <c r="B7" t="str">
-        <v>Unchanged</v>
+        <v>Modified</v>
       </c>
       <c r="C7" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>classAccesses.Send_Email_Confirmation</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.Error_Message__c</v>
       </c>
       <c r="B8" t="str">
-        <v>Changed</v>
+        <v>Modified</v>
       </c>
       <c r="C8" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>tabSettings.Job_Request__c</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.Exception_Details__c</v>
       </c>
       <c r="B9" t="str">
-        <v>Unchanged</v>
+        <v>Modified</v>
       </c>
       <c r="C9" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>recordTypeVisibilities.Recruiting.DevManager</v>
+        <v>fieldPermissions.HIP_API_Transaction__c.Exception_Type__c</v>
       </c>
       <c r="B10" t="str">
-        <v>Unchanged</v>
+        <v>Modified</v>
       </c>
       <c r="C10" t="str">
-        <v>Admin-Passport.xml, Admin-TRV.xml</v>
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.External_Id_Field__c</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.External_Id__c</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Http_Method__c</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Individual_Application__c</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Is_Cached__c</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Level__c</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Log_Generated_Time__c</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Message__c</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Module__c</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Object_Name__c</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Origin__c</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Parent_Request_Id__c</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Record_Id__c</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Request_Id__c</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Request__c</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Response__c</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Running_User__c</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Stack_Trace__c</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.StatusCode__c</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Status__c</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Trace_Id__c</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Transaction_End_Time__c</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Transaction_Logs__c</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Transaction_Start_Time__c</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Transaction_Time_Spent_Milliseconds__c</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Transaction_Type__c</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.Type_Name__c</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.UTC_End_Time_System__c</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>fieldPermissions.HIP_API_Transaction__c.UTC_Start_Time_System__c</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data is getting retrieved to Front-End
</commit_message>
<xml_diff>
--- a/backend/changes.xlsx
+++ b/backend/changes.xlsx
@@ -397,13 +397,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>field</v>
+      </c>
+      <c r="B1" t="str">
+        <v>change</v>
+      </c>
+      <c r="C1" t="str">
+        <v>file</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>0</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>10</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>11</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>12</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>13</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>14</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>15</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>16</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>17</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>18</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>19</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>20</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>21</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>22</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>23</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>24</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>25</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>26</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>27</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>28</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>29</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>30</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>31</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>32</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>33</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>34</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>35</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>36</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>37</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Modified</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Passport_API_Transactions_Read_Only.permissionset-meta.xml, TRV_API_Transactions_Read_Only.permissionset-meta.xml</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>